<commit_message>
Update for Finnish manual
</commit_message>
<xml_diff>
--- a/m52 PnP/Rev1.3 documents/BOM-speeduino v0.4.3 compatible PCB for m52 rev1.3.xlsx
+++ b/m52 PnP/Rev1.3 documents/BOM-speeduino v0.4.3 compatible PCB for m52 rev1.3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kemppain\Documents\GitHub\Speeduino-M5x-PCBs\m52 PnP\Rev1.3 documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m52 PnP\Rev1.3 documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C768C2-84C9-42C4-A088-96934C78828E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E0AD64-1114-4242-888F-E39772FBDDEE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="1695" windowWidth="31680" windowHeight="13380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -1754,14 +1754,14 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2160,8 +2160,8 @@
   </sheetPr>
   <dimension ref="A1:X62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="113" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2871,7 +2871,7 @@
       <c r="M10" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="N10" s="38" t="s">
+      <c r="N10" s="36" t="s">
         <v>318</v>
       </c>
       <c r="O10" s="5">
@@ -3575,7 +3575,7 @@
     </row>
     <row r="21" spans="1:24" ht="16.5" thickBot="1">
       <c r="A21" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" s="18">
         <v>4</v>
@@ -3620,16 +3620,16 @@
       </c>
       <c r="Q21" s="6">
         <f>O21*A21</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R21" s="6">
         <f t="shared" ref="R21" si="12">P21*A21</f>
-        <v>0.88200000000000001</v>
+        <v>1.764</v>
       </c>
       <c r="S21" s="4"/>
       <c r="T21" s="4" t="str">
         <f t="shared" ref="T21" si="13">IF(NOT(M21=""),A21&amp;","&amp;M21,"")</f>
-        <v>1,WM1353-ND</v>
+        <v>2,WM1353-ND</v>
       </c>
       <c r="U21" s="4" t="str">
         <f t="shared" ref="U21" si="14">IF(NOT(M21=""),B21&amp;","&amp;M21,"")</f>
@@ -3637,15 +3637,15 @@
       </c>
       <c r="V21" t="str">
         <f t="shared" ref="V21" si="15">A21&amp;"x "&amp;E21</f>
-        <v>1x 6 POS Header</v>
+        <v>2x 6 POS Header</v>
       </c>
       <c r="W21" t="str">
         <f t="shared" ref="W21" si="16">IF(NOT(N21=""),N21&amp;"|"&amp;A21,"")</f>
-        <v>538-39-30-1060|1</v>
+        <v>538-39-30-1060|2</v>
       </c>
       <c r="X21" t="str">
         <f t="shared" ref="X21" si="17">L21&amp;" "&amp;A21</f>
-        <v>39-30-1060 1</v>
+        <v>39-30-1060 2</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="16.5" thickBot="1">
@@ -5882,10 +5882,10 @@
       <c r="I55" s="8"/>
       <c r="J55" s="4"/>
       <c r="K55" s="8"/>
-      <c r="L55" s="36" t="s">
+      <c r="L55" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="M55" s="37"/>
+      <c r="M55" s="38"/>
       <c r="N55" s="32"/>
       <c r="O55" s="1" t="s">
         <v>68</v>
@@ -5893,11 +5893,11 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="11">
         <f>SUM(Q3:Q50)</f>
-        <v>103.77</v>
+        <v>104.77</v>
       </c>
       <c r="R55" s="11">
         <f>SUM(R3:R50)</f>
-        <v>123.55199999999999</v>
+        <v>124.434</v>
       </c>
       <c r="S55" s="10" t="s">
         <v>69</v>

</xml_diff>